<commit_message>
update push for migrate
</commit_message>
<xml_diff>
--- a/GBS_tables.xlsx
+++ b/GBS_tables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evan/Google Drive/R/GBS_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3779B228-1A66-7643-AE25-4A159B707B8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE662C5-CBA6-3D44-BBBC-DF870281C949}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{769BADEB-7880-FF48-8DF0-084B542D4EC3}"/>
+    <workbookView xWindow="10060" yWindow="6300" windowWidth="25040" windowHeight="14500" activeTab="1" xr2:uid="{769BADEB-7880-FF48-8DF0-084B542D4EC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Pops" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="107">
   <si>
     <t>Mating System</t>
   </si>
@@ -304,16 +305,59 @@
   </si>
   <si>
     <t xml:space="preserve">              1/4</t>
+  </si>
+  <si>
+    <t>B42-S</t>
+  </si>
+  <si>
+    <t>B46-S</t>
+  </si>
+  <si>
+    <t>B49-S</t>
+  </si>
+  <si>
+    <t>B53-S</t>
+  </si>
+  <si>
+    <t>B60-S</t>
+  </si>
+  <si>
+    <t>C59-S</t>
+  </si>
+  <si>
+    <t>L05-S</t>
+  </si>
+  <si>
+    <t>L08-S</t>
+  </si>
+  <si>
+    <t>L10-S</t>
+  </si>
+  <si>
+    <t>L11-S</t>
+  </si>
+  <si>
+    <t>L12-S</t>
+  </si>
+  <si>
+    <t>L13-S</t>
+  </si>
+  <si>
+    <t>L45-S</t>
+  </si>
+  <si>
+    <t>L62-S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -351,7 +395,20 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -404,7 +461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,6 +544,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,17 +870,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D602750B-5FF7-3144-BAF5-2BCD3E35F735}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17" thickBot="1">
+    <row r="1" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +939,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="17" thickTop="1">
+    <row r="2" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -932,7 +998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>10</v>
@@ -987,7 +1053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -1040,7 +1106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>14</v>
@@ -1093,7 +1159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
         <v>16</v>
@@ -1146,7 +1212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>19</v>
@@ -1203,7 +1269,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
         <v>21</v>
@@ -1256,7 +1322,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -1311,7 +1377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
         <v>27</v>
@@ -1364,7 +1430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
         <v>29</v>
@@ -1419,7 +1485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
         <v>31</v>
@@ -1472,7 +1538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
         <v>32</v>
@@ -1527,7 +1593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
         <v>34</v>
@@ -1584,7 +1650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
         <v>35</v>
@@ -1639,7 +1705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
         <v>37</v>
@@ -1694,7 +1760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
         <v>39</v>
@@ -1751,7 +1817,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
         <v>42</v>
@@ -1804,7 +1870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
         <v>44</v>
@@ -1857,7 +1923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
         <v>47</v>
@@ -1910,7 +1976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
         <v>49</v>
@@ -1963,7 +2029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="9" t="s">
         <v>52</v>
@@ -2016,7 +2082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H23" s="16" t="s">
         <v>60</v>
       </c>
@@ -2053,7 +2119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H24" s="16" t="s">
         <v>60</v>
       </c>
@@ -2090,7 +2156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H25" s="16" t="s">
         <v>60</v>
       </c>
@@ -2129,7 +2195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H26" s="16" t="s">
         <v>60</v>
       </c>
@@ -2166,7 +2232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H27" s="16" t="s">
         <v>60</v>
       </c>
@@ -2205,7 +2271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H28" s="16" t="s">
         <v>60</v>
       </c>
@@ -2244,7 +2310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H29" s="16" t="s">
         <v>60</v>
       </c>
@@ -2264,7 +2330,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H30" s="16" t="s">
         <v>60</v>
       </c>
@@ -2281,7 +2347,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="H31" s="16" t="s">
         <v>60</v>
       </c>
@@ -2307,4 +2373,586 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A80760-A1A2-FF44-988F-B8D08259BFEB}">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+    </row>
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="42"/>
+      <c r="B3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="36"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="39">
+        <v>0.16510559999999999</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="36"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="39">
+        <v>0.2029861</v>
+      </c>
+      <c r="C6" s="37">
+        <v>0.17966180000000001</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="36"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="39">
+        <v>0.13166559999999999</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0.16072839999999999</v>
+      </c>
+      <c r="D7" s="37">
+        <v>0.19949529999999999</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="36"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="39">
+        <v>0.15600359999999999</v>
+      </c>
+      <c r="C8" s="37">
+        <v>0.1878109</v>
+      </c>
+      <c r="D8" s="37">
+        <v>0.22645319999999999</v>
+      </c>
+      <c r="E8" s="37">
+        <v>0.1463006</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="36"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="39">
+        <v>0.34618019999999999</v>
+      </c>
+      <c r="C9" s="37">
+        <v>0.3280962</v>
+      </c>
+      <c r="D9" s="37">
+        <v>0.34298810000000002</v>
+      </c>
+      <c r="E9" s="37">
+        <v>0.33656079999999999</v>
+      </c>
+      <c r="F9" s="37">
+        <v>0.3710851</v>
+      </c>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="36"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="39">
+        <v>0.1918754</v>
+      </c>
+      <c r="C10" s="37">
+        <v>0.1706491</v>
+      </c>
+      <c r="D10" s="37">
+        <v>0.15853809999999999</v>
+      </c>
+      <c r="E10" s="37">
+        <v>0.1894477</v>
+      </c>
+      <c r="F10" s="37">
+        <v>0.21663959999999999</v>
+      </c>
+      <c r="G10" s="37">
+        <v>0.31909359999999998</v>
+      </c>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="36"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="39">
+        <v>0.1774879</v>
+      </c>
+      <c r="C11" s="37">
+        <v>0.1553804</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0.147707</v>
+      </c>
+      <c r="E11" s="37">
+        <v>0.1773738</v>
+      </c>
+      <c r="F11" s="37">
+        <v>0.2035093</v>
+      </c>
+      <c r="G11" s="37">
+        <v>0.30606909999999998</v>
+      </c>
+      <c r="H11" s="37">
+        <v>0.1264248</v>
+      </c>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="39">
+        <v>0.16709260000000001</v>
+      </c>
+      <c r="C12" s="37">
+        <v>0.14591129999999999</v>
+      </c>
+      <c r="D12" s="37">
+        <v>0.13947619999999999</v>
+      </c>
+      <c r="E12" s="37">
+        <v>0.1656473</v>
+      </c>
+      <c r="F12" s="37">
+        <v>0.19129650000000001</v>
+      </c>
+      <c r="G12" s="37">
+        <v>0.295433</v>
+      </c>
+      <c r="H12" s="37">
+        <v>0.1210102</v>
+      </c>
+      <c r="I12" s="37">
+        <v>0.11067879</v>
+      </c>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="36"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="39">
+        <v>0.16331519999999999</v>
+      </c>
+      <c r="C13" s="37">
+        <v>0.14071790000000001</v>
+      </c>
+      <c r="D13" s="37">
+        <v>0.1385391</v>
+      </c>
+      <c r="E13" s="37">
+        <v>0.16022130000000001</v>
+      </c>
+      <c r="F13" s="37">
+        <v>0.1887875</v>
+      </c>
+      <c r="G13" s="37">
+        <v>0.29656139999999998</v>
+      </c>
+      <c r="H13" s="37">
+        <v>0.119323</v>
+      </c>
+      <c r="I13" s="37">
+        <v>0.10604863</v>
+      </c>
+      <c r="J13" s="37">
+        <v>0.10214716</v>
+      </c>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="36"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="39">
+        <v>0.17649290000000001</v>
+      </c>
+      <c r="C14" s="37">
+        <v>0.15210370000000001</v>
+      </c>
+      <c r="D14" s="37">
+        <v>0.1447377</v>
+      </c>
+      <c r="E14" s="37">
+        <v>0.17335600000000001</v>
+      </c>
+      <c r="F14" s="37">
+        <v>0.19860030000000001</v>
+      </c>
+      <c r="G14" s="37">
+        <v>0.30112369999999999</v>
+      </c>
+      <c r="H14" s="37">
+        <v>0.1249097</v>
+      </c>
+      <c r="I14" s="37">
+        <v>0.11915317</v>
+      </c>
+      <c r="J14" s="37">
+        <v>0.11144245999999999</v>
+      </c>
+      <c r="K14" s="37">
+        <v>0.10525888</v>
+      </c>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="39">
+        <v>0.1773651</v>
+      </c>
+      <c r="C15" s="37">
+        <v>0.1559912</v>
+      </c>
+      <c r="D15" s="37">
+        <v>0.143371</v>
+      </c>
+      <c r="E15" s="37">
+        <v>0.1751221</v>
+      </c>
+      <c r="F15" s="37">
+        <v>0.20075750000000001</v>
+      </c>
+      <c r="G15" s="37">
+        <v>0.30243330000000002</v>
+      </c>
+      <c r="H15" s="37">
+        <v>0.1268772</v>
+      </c>
+      <c r="I15" s="37">
+        <v>0.11505644</v>
+      </c>
+      <c r="J15" s="37">
+        <v>0.10935639</v>
+      </c>
+      <c r="K15" s="37">
+        <v>0.10483099999999999</v>
+      </c>
+      <c r="L15" s="37">
+        <v>0.10747107</v>
+      </c>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="36"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="39">
+        <v>0.27176460000000002</v>
+      </c>
+      <c r="C16" s="37">
+        <v>0.25700489999999998</v>
+      </c>
+      <c r="D16" s="37">
+        <v>0.25747249999999999</v>
+      </c>
+      <c r="E16" s="37">
+        <v>0.26502999999999999</v>
+      </c>
+      <c r="F16" s="37">
+        <v>0.29465409999999997</v>
+      </c>
+      <c r="G16" s="37">
+        <v>0.29311290000000001</v>
+      </c>
+      <c r="H16" s="37">
+        <v>0.24236199999999999</v>
+      </c>
+      <c r="I16" s="37">
+        <v>0.22940679999999999</v>
+      </c>
+      <c r="J16" s="37">
+        <v>0.21886170999999999</v>
+      </c>
+      <c r="K16" s="37">
+        <v>0.20828587000000001</v>
+      </c>
+      <c r="L16" s="37">
+        <v>0.23014667</v>
+      </c>
+      <c r="M16" s="37">
+        <v>0.22858651999999999</v>
+      </c>
+      <c r="N16" s="37"/>
+      <c r="O16" s="36"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="41">
+        <v>0.15185409999999999</v>
+      </c>
+      <c r="C17" s="41">
+        <v>0.13267570000000001</v>
+      </c>
+      <c r="D17" s="41">
+        <v>0.1251794</v>
+      </c>
+      <c r="E17" s="41">
+        <v>0.15274219999999999</v>
+      </c>
+      <c r="F17" s="41">
+        <v>0.17347489999999999</v>
+      </c>
+      <c r="G17" s="41">
+        <v>0.2719724</v>
+      </c>
+      <c r="H17" s="41">
+        <v>0.1113512</v>
+      </c>
+      <c r="I17" s="41">
+        <v>9.755403E-2</v>
+      </c>
+      <c r="J17" s="41">
+        <v>9.3538319999999994E-2</v>
+      </c>
+      <c r="K17" s="41">
+        <v>8.7383450000000001E-2</v>
+      </c>
+      <c r="L17" s="41">
+        <v>9.4245170000000003E-2</v>
+      </c>
+      <c r="M17" s="41">
+        <v>9.6137120000000006E-2</v>
+      </c>
+      <c r="N17" s="41">
+        <v>0.18498619999999999</v>
+      </c>
+      <c r="O17" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>